<commit_message>
Finalize file with updated districts/complete data
</commit_message>
<xml_diff>
--- a/data/final/public/Baltimore_City/primary_election_2020/Leg_and_Council_Data_by_Precinct revised.xlsx
+++ b/data/final/public/Baltimore_City/primary_election_2020/Leg_and_Council_Data_by_Precinct revised.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lklein26/Documents/GitHub/BCDS_LWV_2023/data/final/public/Baltimore_City/primary_election_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6EA65614-9C8D-3048-9322-07AE03A1019C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C85968-D8F4-BB4C-8C56-72BC1D0C4159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leg_and_Council_Data_by_Precinc" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Leg_and_Council_Data_by_Precinc!$A$1:$BA$300</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="351">
   <si>
     <t>Leg_Dist_Precinct</t>
   </si>
@@ -401,9 +404,6 @@
   </si>
   <si>
     <t>12-013</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>13-001</t>
@@ -1081,7 +1081,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1915,11 +1915,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Z186" sqref="Z186"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14075,86 +14075,86 @@
       <c r="Z76">
         <v>14</v>
       </c>
-      <c r="AA76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AI76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AX76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY76" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ76" t="s">
-        <v>127</v>
-      </c>
-      <c r="BA76" t="s">
-        <v>127</v>
+      <c r="AA76">
+        <v>29.7</v>
+      </c>
+      <c r="AB76">
+        <v>34.25</v>
+      </c>
+      <c r="AC76">
+        <v>115.32</v>
+      </c>
+      <c r="AD76">
+        <v>4.83</v>
+      </c>
+      <c r="AE76">
+        <v>59.01</v>
+      </c>
+      <c r="AF76">
+        <v>40.92</v>
+      </c>
+      <c r="AG76">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AH76">
+        <v>0.2</v>
+      </c>
+      <c r="AI76">
+        <v>11.17</v>
+      </c>
+      <c r="AJ76">
+        <v>31</v>
+      </c>
+      <c r="AK76">
+        <v>21.82</v>
+      </c>
+      <c r="AL76">
+        <v>30.71</v>
+      </c>
+      <c r="AM76">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AN76">
+        <v>53.94</v>
+      </c>
+      <c r="AO76">
+        <v>45.88</v>
+      </c>
+      <c r="AP76">
+        <v>0.18</v>
+      </c>
+      <c r="AQ76">
+        <v>0.31</v>
+      </c>
+      <c r="AR76">
+        <v>15.42</v>
+      </c>
+      <c r="AS76">
+        <v>37.29</v>
+      </c>
+      <c r="AT76">
+        <v>19.18</v>
+      </c>
+      <c r="AU76">
+        <v>27.72</v>
+      </c>
+      <c r="AV76">
+        <v>0.08</v>
+      </c>
+      <c r="AW76">
+        <v>97.82</v>
+      </c>
+      <c r="AX76">
+        <v>1.83</v>
+      </c>
+      <c r="AY76">
+        <v>0.34</v>
+      </c>
+      <c r="AZ76">
+        <v>4</v>
+      </c>
+      <c r="BA76">
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:53" x14ac:dyDescent="0.2">
@@ -14162,7 +14162,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C77">
         <v>41</v>
@@ -14323,7 +14323,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C78">
         <v>40</v>
@@ -14484,7 +14484,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C79">
         <v>40</v>
@@ -14645,7 +14645,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C80">
         <v>40</v>
@@ -14806,7 +14806,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C81">
         <v>40</v>
@@ -14967,7 +14967,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C82">
         <v>40</v>
@@ -15128,7 +15128,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C83">
         <v>40</v>
@@ -15289,7 +15289,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C84">
         <v>40</v>
@@ -15450,7 +15450,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C85">
         <v>40</v>
@@ -15611,7 +15611,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C86">
         <v>40</v>
@@ -15772,7 +15772,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C87">
         <v>43</v>
@@ -15933,7 +15933,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C88">
         <v>40</v>
@@ -16094,7 +16094,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C89">
         <v>40</v>
@@ -16168,86 +16168,86 @@
       <c r="Z89">
         <v>14</v>
       </c>
-      <c r="AA89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AI89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AX89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY89" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ89" t="s">
-        <v>127</v>
-      </c>
-      <c r="BA89" t="s">
-        <v>127</v>
+      <c r="AA89">
+        <v>29.7</v>
+      </c>
+      <c r="AB89">
+        <v>34.25</v>
+      </c>
+      <c r="AC89">
+        <v>115.32</v>
+      </c>
+      <c r="AD89">
+        <v>4.83</v>
+      </c>
+      <c r="AE89">
+        <v>59.01</v>
+      </c>
+      <c r="AF89">
+        <v>40.92</v>
+      </c>
+      <c r="AG89">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AH89">
+        <v>0.2</v>
+      </c>
+      <c r="AI89">
+        <v>11.17</v>
+      </c>
+      <c r="AJ89">
+        <v>31</v>
+      </c>
+      <c r="AK89">
+        <v>21.82</v>
+      </c>
+      <c r="AL89">
+        <v>30.71</v>
+      </c>
+      <c r="AM89">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AN89">
+        <v>53.94</v>
+      </c>
+      <c r="AO89">
+        <v>45.88</v>
+      </c>
+      <c r="AP89">
+        <v>0.18</v>
+      </c>
+      <c r="AQ89">
+        <v>0.31</v>
+      </c>
+      <c r="AR89">
+        <v>15.42</v>
+      </c>
+      <c r="AS89">
+        <v>37.29</v>
+      </c>
+      <c r="AT89">
+        <v>19.18</v>
+      </c>
+      <c r="AU89">
+        <v>27.72</v>
+      </c>
+      <c r="AV89">
+        <v>0.08</v>
+      </c>
+      <c r="AW89">
+        <v>97.82</v>
+      </c>
+      <c r="AX89">
+        <v>1.83</v>
+      </c>
+      <c r="AY89">
+        <v>0.34</v>
+      </c>
+      <c r="AZ89">
+        <v>4</v>
+      </c>
+      <c r="BA89">
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:53" x14ac:dyDescent="0.2">
@@ -16255,7 +16255,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C90">
         <v>40</v>
@@ -16416,7 +16416,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C91">
         <v>40</v>
@@ -16577,7 +16577,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C92">
         <v>44</v>
@@ -16738,7 +16738,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C93">
         <v>44</v>
@@ -16899,7 +16899,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C94">
         <v>40</v>
@@ -17060,7 +17060,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C95">
         <v>41</v>
@@ -17221,7 +17221,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C96">
         <v>41</v>
@@ -17382,7 +17382,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C97">
         <v>41</v>
@@ -17543,7 +17543,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C98">
         <v>40</v>
@@ -17704,7 +17704,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C99">
         <v>40</v>
@@ -17865,7 +17865,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C100">
         <v>40</v>
@@ -18026,7 +18026,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C101">
         <v>41</v>
@@ -18187,7 +18187,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C102">
         <v>41</v>
@@ -18348,7 +18348,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C103">
         <v>41</v>
@@ -18509,7 +18509,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C104">
         <v>41</v>
@@ -18670,7 +18670,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C105">
         <v>41</v>
@@ -18831,7 +18831,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C106">
         <v>41</v>
@@ -18992,7 +18992,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C107">
         <v>40</v>
@@ -19153,7 +19153,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C108">
         <v>40</v>
@@ -19314,7 +19314,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C109">
         <v>40</v>
@@ -19475,7 +19475,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C110">
         <v>40</v>
@@ -19636,7 +19636,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C111">
         <v>40</v>
@@ -19797,7 +19797,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C112">
         <v>40</v>
@@ -19958,7 +19958,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C113">
         <v>44</v>
@@ -20119,7 +20119,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C114">
         <v>40</v>
@@ -20280,7 +20280,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C115">
         <v>40</v>
@@ -20441,7 +20441,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C116">
         <v>40</v>
@@ -20602,7 +20602,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C117">
         <v>40</v>
@@ -20763,7 +20763,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C118">
         <v>40</v>
@@ -20924,7 +20924,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C119">
         <v>40</v>
@@ -21085,7 +21085,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C120">
         <v>44</v>
@@ -21246,7 +21246,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C121">
         <v>40</v>
@@ -21407,7 +21407,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C122">
         <v>44</v>
@@ -21568,7 +21568,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C123">
         <v>44</v>
@@ -21729,7 +21729,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C124">
         <v>44</v>
@@ -21890,7 +21890,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C125">
         <v>40</v>
@@ -22051,7 +22051,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C126">
         <v>44</v>
@@ -22212,7 +22212,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C127">
         <v>40</v>
@@ -22373,7 +22373,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C128">
         <v>40</v>
@@ -22534,7 +22534,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C129">
         <v>40</v>
@@ -22695,7 +22695,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C130">
         <v>40</v>
@@ -22856,7 +22856,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C131">
         <v>40</v>
@@ -23017,7 +23017,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C132">
         <v>41</v>
@@ -23178,7 +23178,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C133">
         <v>41</v>
@@ -23339,7 +23339,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C134">
         <v>44</v>
@@ -23500,7 +23500,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C135">
         <v>40</v>
@@ -23661,7 +23661,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C136">
         <v>40</v>
@@ -23822,7 +23822,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C137">
         <v>40</v>
@@ -23983,7 +23983,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C138">
         <v>44</v>
@@ -24144,7 +24144,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C139">
         <v>40</v>
@@ -24305,7 +24305,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C140">
         <v>44</v>
@@ -24466,7 +24466,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C141">
         <v>44</v>
@@ -24627,7 +24627,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C142">
         <v>44</v>
@@ -24788,7 +24788,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C143">
         <v>44</v>
@@ -24949,7 +24949,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C144">
         <v>44</v>
@@ -25110,7 +25110,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C145">
         <v>41</v>
@@ -25271,7 +25271,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C146">
         <v>41</v>
@@ -25432,7 +25432,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C147">
         <v>41</v>
@@ -25593,7 +25593,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C148">
         <v>44</v>
@@ -25754,7 +25754,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C149">
         <v>44</v>
@@ -25915,7 +25915,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C150">
         <v>40</v>
@@ -26076,7 +26076,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C151">
         <v>40</v>
@@ -26237,7 +26237,7 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C152">
         <v>40</v>
@@ -26311,86 +26311,86 @@
       <c r="Z152">
         <v>10</v>
       </c>
-      <c r="AA152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AI152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AX152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY152" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ152" t="s">
-        <v>127</v>
-      </c>
-      <c r="BA152" t="s">
-        <v>127</v>
+      <c r="AA152">
+        <v>18.93</v>
+      </c>
+      <c r="AB152">
+        <v>18.510000000000002</v>
+      </c>
+      <c r="AC152">
+        <v>97.78</v>
+      </c>
+      <c r="AD152">
+        <v>14.17</v>
+      </c>
+      <c r="AE152">
+        <v>61.34</v>
+      </c>
+      <c r="AF152">
+        <v>38.630000000000003</v>
+      </c>
+      <c r="AG152">
+        <v>0.03</v>
+      </c>
+      <c r="AH152">
+        <v>0.05</v>
+      </c>
+      <c r="AI152">
+        <v>12.87</v>
+      </c>
+      <c r="AJ152">
+        <v>26.64</v>
+      </c>
+      <c r="AK152">
+        <v>30.57</v>
+      </c>
+      <c r="AL152">
+        <v>24.61</v>
+      </c>
+      <c r="AM152">
+        <v>5.26</v>
+      </c>
+      <c r="AN152">
+        <v>54.05</v>
+      </c>
+      <c r="AO152">
+        <v>45.82</v>
+      </c>
+      <c r="AP152">
+        <v>0.12</v>
+      </c>
+      <c r="AQ152">
+        <v>0.32</v>
+      </c>
+      <c r="AR152">
+        <v>16.760000000000002</v>
+      </c>
+      <c r="AS152">
+        <v>34.64</v>
+      </c>
+      <c r="AT152">
+        <v>24.28</v>
+      </c>
+      <c r="AU152">
+        <v>23.82</v>
+      </c>
+      <c r="AV152">
+        <v>0.17</v>
+      </c>
+      <c r="AW152">
+        <v>95.09</v>
+      </c>
+      <c r="AX152">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="AY152">
+        <v>0.64</v>
+      </c>
+      <c r="AZ152">
+        <v>9</v>
+      </c>
+      <c r="BA152">
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:53" x14ac:dyDescent="0.2">
@@ -26398,7 +26398,7 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C153">
         <v>40</v>
@@ -26559,7 +26559,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C154">
         <v>40</v>
@@ -26720,7 +26720,7 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C155">
         <v>40</v>
@@ -26881,7 +26881,7 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C156">
         <v>46</v>
@@ -27042,7 +27042,7 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C157">
         <v>46</v>
@@ -27116,86 +27116,86 @@
       <c r="Z157">
         <v>11</v>
       </c>
-      <c r="AA157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AI157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AX157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY157" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ157" t="s">
-        <v>127</v>
-      </c>
-      <c r="BA157" t="s">
-        <v>127</v>
+      <c r="AA157">
+        <v>21.41</v>
+      </c>
+      <c r="AB157">
+        <v>25.87</v>
+      </c>
+      <c r="AC157">
+        <v>120.81</v>
+      </c>
+      <c r="AD157">
+        <v>4.88</v>
+      </c>
+      <c r="AE157">
+        <v>55.88</v>
+      </c>
+      <c r="AF157">
+        <v>43.98</v>
+      </c>
+      <c r="AG157">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AH157">
+        <v>0.13</v>
+      </c>
+      <c r="AI157">
+        <v>19.37</v>
+      </c>
+      <c r="AJ157">
+        <v>31.66</v>
+      </c>
+      <c r="AK157">
+        <v>20.87</v>
+      </c>
+      <c r="AL157">
+        <v>22.31</v>
+      </c>
+      <c r="AM157">
+        <v>5.65</v>
+      </c>
+      <c r="AN157">
+        <v>51.62</v>
+      </c>
+      <c r="AO157">
+        <v>48.21</v>
+      </c>
+      <c r="AP157">
+        <v>0.17</v>
+      </c>
+      <c r="AQ157">
+        <v>0.19</v>
+      </c>
+      <c r="AR157">
+        <v>20.64</v>
+      </c>
+      <c r="AS157">
+        <v>42.16</v>
+      </c>
+      <c r="AT157">
+        <v>17.62</v>
+      </c>
+      <c r="AU157">
+        <v>19.309999999999999</v>
+      </c>
+      <c r="AV157">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AW157">
+        <v>97.82</v>
+      </c>
+      <c r="AX157">
+        <v>1.91</v>
+      </c>
+      <c r="AY157">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AZ157">
+        <v>1</v>
+      </c>
+      <c r="BA157">
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:53" x14ac:dyDescent="0.2">
@@ -27203,7 +27203,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C158">
         <v>46</v>
@@ -27364,7 +27364,7 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C159">
         <v>46</v>
@@ -27525,7 +27525,7 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C160">
         <v>46</v>
@@ -27686,7 +27686,7 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C161">
         <v>46</v>
@@ -27847,7 +27847,7 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C162">
         <v>46</v>
@@ -28008,7 +28008,7 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C163">
         <v>46</v>
@@ -28169,7 +28169,7 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C164">
         <v>46</v>
@@ -28330,7 +28330,7 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C165">
         <v>46</v>
@@ -28491,7 +28491,7 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C166">
         <v>46</v>
@@ -28652,7 +28652,7 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C167">
         <v>46</v>
@@ -28813,7 +28813,7 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C168">
         <v>44</v>
@@ -28974,7 +28974,7 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C169">
         <v>44</v>
@@ -29135,7 +29135,7 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C170">
         <v>40</v>
@@ -29296,7 +29296,7 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C171">
         <v>40</v>
@@ -29457,7 +29457,7 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C172">
         <v>46</v>
@@ -29618,7 +29618,7 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C173">
         <v>46</v>
@@ -29779,7 +29779,7 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C174">
         <v>46</v>
@@ -29940,7 +29940,7 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C175">
         <v>46</v>
@@ -30101,7 +30101,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C176">
         <v>46</v>
@@ -30262,7 +30262,7 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C177">
         <v>46</v>
@@ -30423,7 +30423,7 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C178">
         <v>46</v>
@@ -30584,7 +30584,7 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C179">
         <v>46</v>
@@ -30745,7 +30745,7 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C180">
         <v>46</v>
@@ -30906,7 +30906,7 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C181">
         <v>46</v>
@@ -31067,7 +31067,7 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C182">
         <v>46</v>
@@ -31228,7 +31228,7 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C183">
         <v>46</v>
@@ -31389,7 +31389,7 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C184">
         <v>40</v>
@@ -31550,7 +31550,7 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C185">
         <v>40</v>
@@ -31624,86 +31624,86 @@
       <c r="Z185">
         <v>10</v>
       </c>
-      <c r="AA185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AI185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AV185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AX185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY185" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ185" t="s">
-        <v>127</v>
-      </c>
-      <c r="BA185" t="s">
-        <v>127</v>
+      <c r="AA185">
+        <v>18.93</v>
+      </c>
+      <c r="AB185">
+        <v>18.510000000000002</v>
+      </c>
+      <c r="AC185">
+        <v>97.78</v>
+      </c>
+      <c r="AD185">
+        <v>14.17</v>
+      </c>
+      <c r="AE185">
+        <v>61.34</v>
+      </c>
+      <c r="AF185">
+        <v>38.630000000000003</v>
+      </c>
+      <c r="AG185">
+        <v>0.03</v>
+      </c>
+      <c r="AH185">
+        <v>0.05</v>
+      </c>
+      <c r="AI185">
+        <v>12.87</v>
+      </c>
+      <c r="AJ185">
+        <v>26.64</v>
+      </c>
+      <c r="AK185">
+        <v>30.57</v>
+      </c>
+      <c r="AL185">
+        <v>24.61</v>
+      </c>
+      <c r="AM185">
+        <v>5.26</v>
+      </c>
+      <c r="AN185">
+        <v>54.05</v>
+      </c>
+      <c r="AO185">
+        <v>45.82</v>
+      </c>
+      <c r="AP185">
+        <v>0.12</v>
+      </c>
+      <c r="AQ185">
+        <v>0.32</v>
+      </c>
+      <c r="AR185">
+        <v>16.760000000000002</v>
+      </c>
+      <c r="AS185">
+        <v>34.64</v>
+      </c>
+      <c r="AT185">
+        <v>24.28</v>
+      </c>
+      <c r="AU185">
+        <v>23.82</v>
+      </c>
+      <c r="AV185">
+        <v>0.17</v>
+      </c>
+      <c r="AW185">
+        <v>95.09</v>
+      </c>
+      <c r="AX185">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="AY185">
+        <v>0.64</v>
+      </c>
+      <c r="AZ185">
+        <v>9</v>
+      </c>
+      <c r="BA185">
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:53" x14ac:dyDescent="0.2">
@@ -31711,7 +31711,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C186">
         <v>46</v>
@@ -31872,7 +31872,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C187">
         <v>46</v>
@@ -32033,7 +32033,7 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C188">
         <v>46</v>
@@ -32194,7 +32194,7 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C189">
         <v>46</v>
@@ -32355,7 +32355,7 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C190">
         <v>46</v>
@@ -32516,7 +32516,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C191">
         <v>46</v>
@@ -32677,7 +32677,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C192">
         <v>46</v>
@@ -32838,7 +32838,7 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C193">
         <v>46</v>
@@ -32999,7 +32999,7 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C194">
         <v>46</v>
@@ -33160,7 +33160,7 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C195">
         <v>46</v>
@@ -33321,7 +33321,7 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C196">
         <v>46</v>
@@ -33482,7 +33482,7 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C197">
         <v>46</v>
@@ -33643,7 +33643,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C198">
         <v>45</v>
@@ -33804,7 +33804,7 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C199">
         <v>45</v>
@@ -33965,7 +33965,7 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C200">
         <v>45</v>
@@ -34126,7 +34126,7 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C201">
         <v>45</v>
@@ -34287,7 +34287,7 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C202">
         <v>45</v>
@@ -34448,7 +34448,7 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C203">
         <v>45</v>
@@ -34609,7 +34609,7 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C204">
         <v>45</v>
@@ -34770,7 +34770,7 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C205">
         <v>45</v>
@@ -34931,7 +34931,7 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C206">
         <v>45</v>
@@ -35092,7 +35092,7 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C207">
         <v>45</v>
@@ -35253,7 +35253,7 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C208">
         <v>45</v>
@@ -35414,7 +35414,7 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C209">
         <v>45</v>
@@ -35575,7 +35575,7 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C210">
         <v>45</v>
@@ -35736,7 +35736,7 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C211">
         <v>45</v>
@@ -35897,7 +35897,7 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C212">
         <v>45</v>
@@ -36058,7 +36058,7 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C213">
         <v>45</v>
@@ -36219,7 +36219,7 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C214">
         <v>45</v>
@@ -36380,7 +36380,7 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C215">
         <v>45</v>
@@ -36541,7 +36541,7 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C216">
         <v>45</v>
@@ -36702,7 +36702,7 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C217">
         <v>45</v>
@@ -36863,7 +36863,7 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C218">
         <v>45</v>
@@ -37024,7 +37024,7 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C219">
         <v>45</v>
@@ -37185,7 +37185,7 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C220">
         <v>45</v>
@@ -37346,7 +37346,7 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C221">
         <v>45</v>
@@ -37507,7 +37507,7 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C222">
         <v>45</v>
@@ -37668,7 +37668,7 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C223">
         <v>45</v>
@@ -37829,7 +37829,7 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C224">
         <v>45</v>
@@ -37990,7 +37990,7 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C225">
         <v>45</v>
@@ -38151,7 +38151,7 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C226">
         <v>45</v>
@@ -38312,7 +38312,7 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C227">
         <v>45</v>
@@ -38473,7 +38473,7 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C228">
         <v>45</v>
@@ -38634,7 +38634,7 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C229">
         <v>45</v>
@@ -38795,7 +38795,7 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C230">
         <v>43</v>
@@ -38956,7 +38956,7 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C231">
         <v>43</v>
@@ -39117,7 +39117,7 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C232">
         <v>45</v>
@@ -39278,7 +39278,7 @@
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C233">
         <v>43</v>
@@ -39439,7 +39439,7 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C234">
         <v>43</v>
@@ -39600,7 +39600,7 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C235">
         <v>43</v>
@@ -39761,7 +39761,7 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C236">
         <v>43</v>
@@ -39922,7 +39922,7 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C237">
         <v>43</v>
@@ -40083,7 +40083,7 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C238">
         <v>43</v>
@@ -40244,7 +40244,7 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C239">
         <v>43</v>
@@ -40405,7 +40405,7 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C240">
         <v>43</v>
@@ -40566,7 +40566,7 @@
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C241">
         <v>43</v>
@@ -40727,7 +40727,7 @@
         <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C242">
         <v>43</v>
@@ -40888,7 +40888,7 @@
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C243">
         <v>43</v>
@@ -41049,7 +41049,7 @@
         <v>243</v>
       </c>
       <c r="B244" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C244">
         <v>43</v>
@@ -41210,7 +41210,7 @@
         <v>244</v>
       </c>
       <c r="B245" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C245">
         <v>43</v>
@@ -41371,7 +41371,7 @@
         <v>245</v>
       </c>
       <c r="B246" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C246">
         <v>43</v>
@@ -41532,7 +41532,7 @@
         <v>246</v>
       </c>
       <c r="B247" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C247">
         <v>43</v>
@@ -41693,7 +41693,7 @@
         <v>247</v>
       </c>
       <c r="B248" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C248">
         <v>43</v>
@@ -41854,7 +41854,7 @@
         <v>248</v>
       </c>
       <c r="B249" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C249">
         <v>43</v>
@@ -42015,7 +42015,7 @@
         <v>249</v>
       </c>
       <c r="B250" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C250">
         <v>43</v>
@@ -42176,7 +42176,7 @@
         <v>250</v>
       </c>
       <c r="B251" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C251">
         <v>43</v>
@@ -42337,7 +42337,7 @@
         <v>251</v>
       </c>
       <c r="B252" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C252">
         <v>43</v>
@@ -42498,7 +42498,7 @@
         <v>252</v>
       </c>
       <c r="B253" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C253">
         <v>43</v>
@@ -42659,7 +42659,7 @@
         <v>253</v>
       </c>
       <c r="B254" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C254">
         <v>43</v>
@@ -42820,7 +42820,7 @@
         <v>254</v>
       </c>
       <c r="B255" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C255">
         <v>43</v>
@@ -42981,7 +42981,7 @@
         <v>255</v>
       </c>
       <c r="B256" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C256">
         <v>43</v>
@@ -43142,7 +43142,7 @@
         <v>256</v>
       </c>
       <c r="B257" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C257">
         <v>43</v>
@@ -43303,7 +43303,7 @@
         <v>257</v>
       </c>
       <c r="B258" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C258">
         <v>43</v>
@@ -43464,7 +43464,7 @@
         <v>258</v>
       </c>
       <c r="B259" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C259">
         <v>43</v>
@@ -43625,7 +43625,7 @@
         <v>259</v>
       </c>
       <c r="B260" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C260">
         <v>41</v>
@@ -43786,7 +43786,7 @@
         <v>260</v>
       </c>
       <c r="B261" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C261">
         <v>41</v>
@@ -43947,7 +43947,7 @@
         <v>261</v>
       </c>
       <c r="B262" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C262">
         <v>41</v>
@@ -44108,7 +44108,7 @@
         <v>262</v>
       </c>
       <c r="B263" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C263">
         <v>41</v>
@@ -44269,7 +44269,7 @@
         <v>263</v>
       </c>
       <c r="B264" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C264">
         <v>41</v>
@@ -44430,7 +44430,7 @@
         <v>264</v>
       </c>
       <c r="B265" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C265">
         <v>41</v>
@@ -44591,7 +44591,7 @@
         <v>265</v>
       </c>
       <c r="B266" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C266">
         <v>41</v>
@@ -44752,7 +44752,7 @@
         <v>266</v>
       </c>
       <c r="B267" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C267">
         <v>41</v>
@@ -44913,7 +44913,7 @@
         <v>267</v>
       </c>
       <c r="B268" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C268">
         <v>41</v>
@@ -45074,7 +45074,7 @@
         <v>268</v>
       </c>
       <c r="B269" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C269">
         <v>41</v>
@@ -45235,7 +45235,7 @@
         <v>269</v>
       </c>
       <c r="B270" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C270">
         <v>41</v>
@@ -45396,7 +45396,7 @@
         <v>270</v>
       </c>
       <c r="B271" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C271">
         <v>40</v>
@@ -45557,7 +45557,7 @@
         <v>271</v>
       </c>
       <c r="B272" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C272">
         <v>40</v>
@@ -45718,7 +45718,7 @@
         <v>272</v>
       </c>
       <c r="B273" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C273">
         <v>41</v>
@@ -45879,7 +45879,7 @@
         <v>273</v>
       </c>
       <c r="B274" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C274">
         <v>41</v>
@@ -46040,7 +46040,7 @@
         <v>274</v>
       </c>
       <c r="B275" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C275">
         <v>41</v>
@@ -46201,7 +46201,7 @@
         <v>275</v>
       </c>
       <c r="B276" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C276">
         <v>41</v>
@@ -46362,7 +46362,7 @@
         <v>276</v>
       </c>
       <c r="B277" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C277">
         <v>41</v>
@@ -46523,7 +46523,7 @@
         <v>277</v>
       </c>
       <c r="B278" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C278">
         <v>41</v>
@@ -46684,7 +46684,7 @@
         <v>278</v>
       </c>
       <c r="B279" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C279">
         <v>41</v>
@@ -46845,7 +46845,7 @@
         <v>279</v>
       </c>
       <c r="B280" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C280">
         <v>41</v>
@@ -47006,7 +47006,7 @@
         <v>280</v>
       </c>
       <c r="B281" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C281">
         <v>41</v>
@@ -47167,7 +47167,7 @@
         <v>281</v>
       </c>
       <c r="B282" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C282">
         <v>41</v>
@@ -47328,7 +47328,7 @@
         <v>282</v>
       </c>
       <c r="B283" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C283">
         <v>41</v>
@@ -47489,7 +47489,7 @@
         <v>283</v>
       </c>
       <c r="B284" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C284">
         <v>41</v>
@@ -47650,7 +47650,7 @@
         <v>284</v>
       </c>
       <c r="B285" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C285">
         <v>41</v>
@@ -47811,7 +47811,7 @@
         <v>285</v>
       </c>
       <c r="B286" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C286">
         <v>41</v>
@@ -47972,7 +47972,7 @@
         <v>286</v>
       </c>
       <c r="B287" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C287">
         <v>41</v>
@@ -48133,7 +48133,7 @@
         <v>287</v>
       </c>
       <c r="B288" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C288">
         <v>41</v>
@@ -48294,7 +48294,7 @@
         <v>288</v>
       </c>
       <c r="B289" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C289">
         <v>41</v>
@@ -48455,7 +48455,7 @@
         <v>289</v>
       </c>
       <c r="B290" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C290">
         <v>41</v>
@@ -48616,7 +48616,7 @@
         <v>290</v>
       </c>
       <c r="B291" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C291">
         <v>41</v>
@@ -48777,7 +48777,7 @@
         <v>291</v>
       </c>
       <c r="B292" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C292">
         <v>41</v>
@@ -48938,7 +48938,7 @@
         <v>292</v>
       </c>
       <c r="B293" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C293">
         <v>41</v>
@@ -49099,7 +49099,7 @@
         <v>293</v>
       </c>
       <c r="B294" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C294">
         <v>41</v>
@@ -49260,7 +49260,7 @@
         <v>294</v>
       </c>
       <c r="B295" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C295">
         <v>41</v>
@@ -49421,7 +49421,7 @@
         <v>295</v>
       </c>
       <c r="B296" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C296">
         <v>41</v>
@@ -49582,7 +49582,7 @@
         <v>296</v>
       </c>
       <c r="B297" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C297">
         <v>41</v>
@@ -49743,7 +49743,7 @@
         <v>297</v>
       </c>
       <c r="B298" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C298">
         <v>44</v>
@@ -49904,7 +49904,7 @@
         <v>298</v>
       </c>
       <c r="B299" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C299">
         <v>44</v>
@@ -50065,7 +50065,7 @@
         <v>299</v>
       </c>
       <c r="B300" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C300">
         <v>41</v>
@@ -50222,6 +50222,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:BA300" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>